<commit_message>
fix MagicPay WebHooks, update layout nomina
</commit_message>
<xml_diff>
--- a/public/boveda/layouts/express_nomina.xlsx
+++ b/public/boveda/layouts/express_nomina.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">Área</t>
   </si>
@@ -49,8 +49,7 @@
     <t xml:space="preserve">Fecha de alta</t>
   </si>
   <si>
-    <t xml:space="preserve">Puesto 
-funcional</t>
+    <t xml:space="preserve">Puesto funcional</t>
   </si>
   <si>
     <t xml:space="preserve">Confianza</t>
@@ -68,6 +67,12 @@
     <t xml:space="preserve">Cuenta</t>
   </si>
   <si>
+    <t xml:space="preserve">Telefono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tecnología</t>
   </si>
   <si>
@@ -77,42 +82,46 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">MALU970621T16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MALU970621HHGGGR02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAGALLON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LUGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">URIEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desarrollador Sr</t>
+    <t xml:space="preserve">XAXX010101000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XEXX010101HNEXXXA4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MERCEDES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEVALLOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desarrollador Jr</t>
   </si>
   <si>
     <t xml:space="preserve">SANTANDER</t>
   </si>
   <si>
-    <t xml:space="preserve">014180567746579655</t>
+    <t xml:space="preserve">014584265147523598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@suempresa.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="[$$-80A]#,##0;\-[$$-80A]#,##0"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-\$* #,##0.00_-;&quot;-$&quot;* #,##0.00_-;_-\$* \-??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -167,6 +176,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -288,38 +304,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -327,15 +339,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -343,7 +355,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -355,23 +367,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="7" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="7" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,7 +383,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,122 +468,142 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O:O"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K7" activeCellId="0" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27.58"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="15.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="3" width="14.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="19.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="19.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="13" t="s">
         <v>14</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="D2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="E2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="19" t="n">
+      <c r="G2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="16" t="n">
         <v>45208</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="20" t="n">
-        <f aca="false">14400*2</f>
-        <v>28800</v>
-      </c>
-      <c r="M2" s="20" t="n">
-        <v>20959.78</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="17" t="s">
+      <c r="J2" s="14" t="s">
         <v>25</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="17" t="n">
+        <v>12000</v>
+      </c>
+      <c r="M2" s="17" t="n">
+        <v>5500</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="1" t="n">
+        <v>5821463275</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q2" r:id="rId1" display="info@suempresa.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>